<commit_message>
Add two tugboats in maintenance
</commit_message>
<xml_diff>
--- a/web/WBTBSsystem/test_tug.xlsx
+++ b/web/WBTBSsystem/test_tug.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YSY\Desktop\GRP\CW\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B999893-3270-4930-BB08-817BB31B7BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A96CD4D-3268-4D2A-B0AA-BA1DE6EDE95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="1800" windowWidth="18840" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>TugBoatId</t>
   </si>
@@ -162,6 +162,22 @@
   </si>
   <si>
     <t>CP0020</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NB021</t>
+  </si>
+  <si>
+    <t>NB022</t>
+  </si>
+  <si>
+    <t>CP0021</t>
+  </si>
+  <si>
+    <t>CP0022</t>
   </si>
 </sst>
 </file>
@@ -545,21 +561,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.453125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -593,7 +609,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -610,7 +626,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -627,7 +643,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -644,7 +660,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -661,12 +677,12 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -678,7 +694,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -695,7 +711,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -712,7 +728,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -729,7 +745,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -746,7 +762,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -763,7 +779,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -780,12 +796,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -797,7 +813,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -814,7 +830,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -831,7 +847,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -848,7 +864,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -865,7 +881,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -882,7 +898,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -899,7 +915,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -913,6 +929,40 @@
         <v>0.375</v>
       </c>
       <c r="E21" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="E23" s="5">
         <v>0.75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit tug boat starting time
</commit_message>
<xml_diff>
--- a/web/WBTBSsystem/test_tug.xlsx
+++ b/web/WBTBSsystem/test_tug.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YSY\Desktop\GRP\CW\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - University of Nottingham Malaysia\Documents\Software GRP\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A96CD4D-3268-4D2A-B0AA-BA1DE6EDE95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E64E441-A52C-4F78-A557-DDFB1A9052E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,11 +184,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -206,7 +206,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -258,7 +258,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,18 +564,18 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -603,13 +603,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="5">
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -620,13 +620,13 @@
         <v>27</v>
       </c>
       <c r="D3" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="5">
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -637,13 +637,13 @@
         <v>28</v>
       </c>
       <c r="D4" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E4" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -654,13 +654,13 @@
         <v>29</v>
       </c>
       <c r="D5" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E5" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -671,13 +671,13 @@
         <v>30</v>
       </c>
       <c r="D6" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E6" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -688,13 +688,13 @@
         <v>31</v>
       </c>
       <c r="D7" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E7" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -705,13 +705,13 @@
         <v>32</v>
       </c>
       <c r="D8" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E8" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -722,13 +722,13 @@
         <v>33</v>
       </c>
       <c r="D9" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E9" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -739,13 +739,13 @@
         <v>34</v>
       </c>
       <c r="D10" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E10" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -756,13 +756,13 @@
         <v>35</v>
       </c>
       <c r="D11" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E11" s="5">
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -773,13 +773,13 @@
         <v>36</v>
       </c>
       <c r="D12" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E12" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -790,13 +790,13 @@
         <v>37</v>
       </c>
       <c r="D13" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E13" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -807,13 +807,13 @@
         <v>38</v>
       </c>
       <c r="D14" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E14" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -824,13 +824,13 @@
         <v>39</v>
       </c>
       <c r="D15" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E15" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -841,13 +841,13 @@
         <v>40</v>
       </c>
       <c r="D16" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E16" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -858,13 +858,13 @@
         <v>41</v>
       </c>
       <c r="D17" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E17" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -875,13 +875,13 @@
         <v>42</v>
       </c>
       <c r="D18" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E18" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -892,13 +892,13 @@
         <v>43</v>
       </c>
       <c r="D19" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E19" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -909,13 +909,13 @@
         <v>44</v>
       </c>
       <c r="D20" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E20" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -926,13 +926,13 @@
         <v>45</v>
       </c>
       <c r="D21" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E21" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -943,13 +943,13 @@
         <v>49</v>
       </c>
       <c r="D22" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E22" s="5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -960,7 +960,7 @@
         <v>50</v>
       </c>
       <c r="D23" s="5">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E23" s="5">
         <v>0.75</v>

</xml_diff>

<commit_message>
Add more 20 tugboats
</commit_message>
<xml_diff>
--- a/web/WBTBSsystem/test_tug.xlsx
+++ b/web/WBTBSsystem/test_tug.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - University of Nottingham Malaysia\Documents\Software GRP\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YSY\Desktop\GRP\CW\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E64E441-A52C-4F78-A557-DDFB1A9052E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0246F6E-66E3-4914-AB7F-9A3B3C0B778F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
   <si>
     <t>TugBoatId</t>
   </si>
@@ -178,17 +178,125 @@
   </si>
   <si>
     <t>CP0022</t>
+  </si>
+  <si>
+    <t>NB023</t>
+  </si>
+  <si>
+    <t>CP0023</t>
+  </si>
+  <si>
+    <t>NB024</t>
+  </si>
+  <si>
+    <t>CP0024</t>
+  </si>
+  <si>
+    <t>NB025</t>
+  </si>
+  <si>
+    <t>CP0025</t>
+  </si>
+  <si>
+    <t>NB026</t>
+  </si>
+  <si>
+    <t>CP0026</t>
+  </si>
+  <si>
+    <t>NB027</t>
+  </si>
+  <si>
+    <t>CP0027</t>
+  </si>
+  <si>
+    <t>NB028</t>
+  </si>
+  <si>
+    <t>CP0028</t>
+  </si>
+  <si>
+    <t>NB029</t>
+  </si>
+  <si>
+    <t>CP0029</t>
+  </si>
+  <si>
+    <t>NB030</t>
+  </si>
+  <si>
+    <t>CP0030</t>
+  </si>
+  <si>
+    <t>NB031</t>
+  </si>
+  <si>
+    <t>CP0031</t>
+  </si>
+  <si>
+    <t>NB032</t>
+  </si>
+  <si>
+    <t>CP0032</t>
+  </si>
+  <si>
+    <t>NB033</t>
+  </si>
+  <si>
+    <t>CP0033</t>
+  </si>
+  <si>
+    <t>NB034</t>
+  </si>
+  <si>
+    <t>CP0034</t>
+  </si>
+  <si>
+    <t>NB035</t>
+  </si>
+  <si>
+    <t>CP0035</t>
+  </si>
+  <si>
+    <t>NB036</t>
+  </si>
+  <si>
+    <t>CP0036</t>
+  </si>
+  <si>
+    <t>NB037</t>
+  </si>
+  <si>
+    <t>CP0037</t>
+  </si>
+  <si>
+    <t>NB038</t>
+  </si>
+  <si>
+    <t>CP0038</t>
+  </si>
+  <si>
+    <t>NB039</t>
+  </si>
+  <si>
+    <t>CP0039</t>
+  </si>
+  <si>
+    <t>NB040</t>
+  </si>
+  <si>
+    <t>CP0040</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -206,7 +314,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -258,7 +366,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -561,21 +669,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -609,7 +717,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -626,7 +734,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -643,7 +751,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -660,7 +768,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -677,7 +785,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -694,7 +802,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -711,7 +819,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -728,7 +836,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -745,7 +853,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -762,7 +870,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -779,7 +887,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -796,7 +904,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -813,7 +921,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -830,7 +938,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -847,7 +955,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -864,7 +972,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -881,7 +989,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -898,7 +1006,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -915,7 +1023,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -932,7 +1040,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -949,7 +1057,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -965,6 +1073,327 @@
       <c r="E23" s="5">
         <v>0.75</v>
       </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B42"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>